<commit_message>
Fixed issues with non-unique headers
Updated to better deal with non-unique headers in spreadsheet
</commit_message>
<xml_diff>
--- a/data/Output1.xlsx
+++ b/data/Output1.xlsx
@@ -430,12 +430,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Column 1</t>
+          <t>Tab 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>New Column 2</t>
+          <t>Tab 1</t>
         </is>
       </c>
     </row>

</xml_diff>